<commit_message>
Trying to push changes
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Baseline.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEDAC2E-33BE-489A-8643-A8474E8096EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC35215-8813-41BE-B1AC-CC457B1CFBB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7668" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +441,7 @@
         <v>12</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -449,7 +449,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>